<commit_message>
update reporting structure agai 3
</commit_message>
<xml_diff>
--- a/reporting_hierarchy.xlsx
+++ b/reporting_hierarchy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29103"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AEE0F21-4041-49D3-A561-5EA1DF1851CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{817AD7FD-10A5-46F9-8341-F5388DB7319B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="257">
   <si>
     <t>Employee No</t>
   </si>
@@ -427,7 +427,7 @@
     <t>Rahul Kalyankar</t>
   </si>
   <si>
-    <t>rahul.kalyankar@urbanagabru.in</t>
+    <t>Rahul.Kalyankar@urbangabru.in</t>
   </si>
   <si>
     <t>Process improvement</t>
@@ -739,6 +739,9 @@
   </si>
   <si>
     <t>shristi.bihani@urbangabru.in</t>
+  </si>
+  <si>
+    <t>Rahul.Kalyankar@urbangabru.co.in</t>
   </si>
   <si>
     <t>Avinash Desale</t>
@@ -1208,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3591,6 +3594,38 @@
       </c>
       <c r="J74" s="1">
         <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1">
+        <v>448</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J75" s="1">
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -3672,48 +3707,50 @@
     <hyperlink ref="D46" r:id="rId74" xr:uid="{65D20DC5-D347-4B92-939D-67C6E9CA4099}"/>
     <hyperlink ref="D47" r:id="rId75" xr:uid="{C53125F8-9352-487F-84D2-E15D4AB7961A}"/>
     <hyperlink ref="D48" r:id="rId76" xr:uid="{DFDBB072-57B6-414E-AD32-C43529C0A02E}"/>
-    <hyperlink ref="D36" r:id="rId77" xr:uid="{3188CB5A-A50C-49D2-93D0-605F6447520C}"/>
-    <hyperlink ref="D34" r:id="rId78" xr:uid="{F32CC1AB-1D08-4CBF-8734-41FE9CE792F2}"/>
-    <hyperlink ref="D37" r:id="rId79" xr:uid="{91939463-F347-4EB1-9835-10D0C5847AC2}"/>
-    <hyperlink ref="D50" r:id="rId80" xr:uid="{697A9CA5-37EE-4DA8-8785-23118AA9A986}"/>
-    <hyperlink ref="D51" r:id="rId81" xr:uid="{B837B941-6C09-4383-8340-057EFEEF4C2A}"/>
-    <hyperlink ref="D53" r:id="rId82" xr:uid="{5228BFFC-0024-4B76-A50F-378E909DEB9E}"/>
-    <hyperlink ref="D56" r:id="rId83" xr:uid="{03A49264-3529-4D46-96B4-F9E4B408275C}"/>
-    <hyperlink ref="D57" r:id="rId84" xr:uid="{B80B62FD-0A48-424D-9193-718DE528A3D9}"/>
-    <hyperlink ref="D60" r:id="rId85" xr:uid="{FF27CE65-EDD1-48CB-ADD2-FC1B04379D4F}"/>
-    <hyperlink ref="D61" r:id="rId86" xr:uid="{DD7177EA-B1A0-4A32-8ECC-126A8F698C87}"/>
-    <hyperlink ref="D62" r:id="rId87" xr:uid="{51AD824A-C8CC-4BDA-BDCB-CACD814337EE}"/>
-    <hyperlink ref="D63" r:id="rId88" xr:uid="{4D20B7EA-6506-4321-91D8-D043FDC215DB}"/>
-    <hyperlink ref="D64" r:id="rId89" xr:uid="{53CA0A1B-9838-4F34-9189-994827F11B4F}"/>
-    <hyperlink ref="D65" r:id="rId90" xr:uid="{006B567B-960D-4976-BA47-34C8AAC2EA6B}"/>
-    <hyperlink ref="D66" r:id="rId91" xr:uid="{D77DFDE8-52D1-47B3-937D-8875B12C8187}"/>
-    <hyperlink ref="D67" r:id="rId92" xr:uid="{4DAD1DCD-6DA4-4821-8767-096D23FA684C}"/>
-    <hyperlink ref="D68" r:id="rId93" xr:uid="{DE32128C-030C-49D8-B6C1-826E021812FC}"/>
-    <hyperlink ref="D69" r:id="rId94" xr:uid="{CBA88F32-2246-46B4-AC53-88544E823387}"/>
-    <hyperlink ref="D70" r:id="rId95" xr:uid="{FC846F3F-D1FA-4F31-B652-3CF29A90246C}"/>
-    <hyperlink ref="D71" r:id="rId96" xr:uid="{BFEFF04B-2141-4567-96A6-D3056766BB0D}"/>
-    <hyperlink ref="I36" r:id="rId97" xr:uid="{A6C0CC82-44BA-4222-B39E-D7476DA47C6B}"/>
-    <hyperlink ref="I59" r:id="rId98" xr:uid="{5DC615E7-939C-43DA-B019-1328E3A6AB38}"/>
-    <hyperlink ref="I14" r:id="rId99" xr:uid="{4C4DDAEE-F389-4B2E-BF3A-B7B53B7D3F87}"/>
-    <hyperlink ref="I34:I35" r:id="rId100" display="shailesh.bhujbal@urbangabru.co.in" xr:uid="{4B015309-8B52-4485-9965-99C88E6F4FAC}"/>
-    <hyperlink ref="I20" r:id="rId101" xr:uid="{E2E655CA-8855-4FFF-8D68-FE7BE3856DAD}"/>
-    <hyperlink ref="I22:I23" r:id="rId102" xr:uid="{249F710E-612E-4A2B-9513-A7E0D75A00F0}"/>
-    <hyperlink ref="I31" r:id="rId103" xr:uid="{0DDB982B-4488-4CAE-AE51-CE129FB8AF5D}"/>
-    <hyperlink ref="I41" r:id="rId104" xr:uid="{6CE8AB3C-163D-40F6-96CD-419E037BC515}"/>
-    <hyperlink ref="I47:I49" r:id="rId105" xr:uid="{49138BDB-FD98-425A-8A09-D467631C7A6C}"/>
-    <hyperlink ref="I56" r:id="rId106" xr:uid="{85529956-96FD-44B7-B1B5-B8B96D656A21}"/>
-    <hyperlink ref="I60" r:id="rId107" xr:uid="{B3890C9C-5043-447C-9BE8-849115F9ED91}"/>
-    <hyperlink ref="I13" r:id="rId108" xr:uid="{B06B408B-86DE-4DC1-A0B1-E651C3474CC0}"/>
-    <hyperlink ref="D72" r:id="rId109" xr:uid="{2BB55C61-927A-4ACD-BFB5-8BFBEB3AB87D}"/>
-    <hyperlink ref="I72" r:id="rId110" xr:uid="{FE4CB666-8CCD-41A4-88DC-772F7E72B69E}"/>
-    <hyperlink ref="I18" r:id="rId111" xr:uid="{65D62495-7ED6-4AEE-85AA-5E06DD4DCC50}"/>
-    <hyperlink ref="I38" r:id="rId112" xr:uid="{5A19F303-21CE-4C85-8F0C-E1C79BC97EE4}"/>
-    <hyperlink ref="I44" r:id="rId113" xr:uid="{CE65FCF0-CAD9-4672-ABBE-37B0F48F2980}"/>
-    <hyperlink ref="I55" r:id="rId114" xr:uid="{EE4F0454-9D7B-4D12-AF17-1357CE1D3E35}"/>
-    <hyperlink ref="I57:I58" r:id="rId115" display="shrushti.mulage@urbangabru.in" xr:uid="{6033AC21-F7BE-4E51-A959-D5962C670FA3}"/>
-    <hyperlink ref="D73" r:id="rId116" xr:uid="{D4FDC315-7B6D-4469-88E3-1589B741FE41}"/>
-    <hyperlink ref="I73" r:id="rId117" xr:uid="{C558B3C7-EBFE-4FB4-ADD6-6EB2E4AD0F9E}"/>
-    <hyperlink ref="I74" r:id="rId118" xr:uid="{D462771F-AC20-49C3-B70C-FA245A6B1D6F}"/>
+    <hyperlink ref="D34" r:id="rId77" xr:uid="{F32CC1AB-1D08-4CBF-8734-41FE9CE792F2}"/>
+    <hyperlink ref="D37" r:id="rId78" xr:uid="{91939463-F347-4EB1-9835-10D0C5847AC2}"/>
+    <hyperlink ref="D50" r:id="rId79" xr:uid="{697A9CA5-37EE-4DA8-8785-23118AA9A986}"/>
+    <hyperlink ref="D51" r:id="rId80" xr:uid="{B837B941-6C09-4383-8340-057EFEEF4C2A}"/>
+    <hyperlink ref="D53" r:id="rId81" xr:uid="{5228BFFC-0024-4B76-A50F-378E909DEB9E}"/>
+    <hyperlink ref="D56" r:id="rId82" xr:uid="{03A49264-3529-4D46-96B4-F9E4B408275C}"/>
+    <hyperlink ref="D57" r:id="rId83" xr:uid="{B80B62FD-0A48-424D-9193-718DE528A3D9}"/>
+    <hyperlink ref="D60" r:id="rId84" xr:uid="{FF27CE65-EDD1-48CB-ADD2-FC1B04379D4F}"/>
+    <hyperlink ref="D61" r:id="rId85" xr:uid="{DD7177EA-B1A0-4A32-8ECC-126A8F698C87}"/>
+    <hyperlink ref="D62" r:id="rId86" xr:uid="{51AD824A-C8CC-4BDA-BDCB-CACD814337EE}"/>
+    <hyperlink ref="D63" r:id="rId87" xr:uid="{4D20B7EA-6506-4321-91D8-D043FDC215DB}"/>
+    <hyperlink ref="D64" r:id="rId88" xr:uid="{53CA0A1B-9838-4F34-9189-994827F11B4F}"/>
+    <hyperlink ref="D65" r:id="rId89" xr:uid="{006B567B-960D-4976-BA47-34C8AAC2EA6B}"/>
+    <hyperlink ref="D66" r:id="rId90" xr:uid="{D77DFDE8-52D1-47B3-937D-8875B12C8187}"/>
+    <hyperlink ref="D67" r:id="rId91" xr:uid="{4DAD1DCD-6DA4-4821-8767-096D23FA684C}"/>
+    <hyperlink ref="D68" r:id="rId92" xr:uid="{DE32128C-030C-49D8-B6C1-826E021812FC}"/>
+    <hyperlink ref="D69" r:id="rId93" xr:uid="{CBA88F32-2246-46B4-AC53-88544E823387}"/>
+    <hyperlink ref="D70" r:id="rId94" xr:uid="{FC846F3F-D1FA-4F31-B652-3CF29A90246C}"/>
+    <hyperlink ref="D71" r:id="rId95" xr:uid="{BFEFF04B-2141-4567-96A6-D3056766BB0D}"/>
+    <hyperlink ref="I36" r:id="rId96" xr:uid="{A6C0CC82-44BA-4222-B39E-D7476DA47C6B}"/>
+    <hyperlink ref="I59" r:id="rId97" xr:uid="{5DC615E7-939C-43DA-B019-1328E3A6AB38}"/>
+    <hyperlink ref="I14" r:id="rId98" xr:uid="{4C4DDAEE-F389-4B2E-BF3A-B7B53B7D3F87}"/>
+    <hyperlink ref="I34:I35" r:id="rId99" display="shailesh.bhujbal@urbangabru.co.in" xr:uid="{4B015309-8B52-4485-9965-99C88E6F4FAC}"/>
+    <hyperlink ref="I20" r:id="rId100" xr:uid="{E2E655CA-8855-4FFF-8D68-FE7BE3856DAD}"/>
+    <hyperlink ref="I22:I23" r:id="rId101" xr:uid="{249F710E-612E-4A2B-9513-A7E0D75A00F0}"/>
+    <hyperlink ref="I31" r:id="rId102" xr:uid="{0DDB982B-4488-4CAE-AE51-CE129FB8AF5D}"/>
+    <hyperlink ref="I41" r:id="rId103" xr:uid="{6CE8AB3C-163D-40F6-96CD-419E037BC515}"/>
+    <hyperlink ref="I47:I49" r:id="rId104" xr:uid="{49138BDB-FD98-425A-8A09-D467631C7A6C}"/>
+    <hyperlink ref="I56" r:id="rId105" xr:uid="{85529956-96FD-44B7-B1B5-B8B96D656A21}"/>
+    <hyperlink ref="I60" r:id="rId106" xr:uid="{B3890C9C-5043-447C-9BE8-849115F9ED91}"/>
+    <hyperlink ref="I13" r:id="rId107" xr:uid="{B06B408B-86DE-4DC1-A0B1-E651C3474CC0}"/>
+    <hyperlink ref="D72" r:id="rId108" xr:uid="{2BB55C61-927A-4ACD-BFB5-8BFBEB3AB87D}"/>
+    <hyperlink ref="I72" r:id="rId109" xr:uid="{FE4CB666-8CCD-41A4-88DC-772F7E72B69E}"/>
+    <hyperlink ref="I18" r:id="rId110" xr:uid="{65D62495-7ED6-4AEE-85AA-5E06DD4DCC50}"/>
+    <hyperlink ref="I38" r:id="rId111" xr:uid="{5A19F303-21CE-4C85-8F0C-E1C79BC97EE4}"/>
+    <hyperlink ref="I44" r:id="rId112" xr:uid="{CE65FCF0-CAD9-4672-ABBE-37B0F48F2980}"/>
+    <hyperlink ref="I55" r:id="rId113" xr:uid="{EE4F0454-9D7B-4D12-AF17-1357CE1D3E35}"/>
+    <hyperlink ref="I57:I58" r:id="rId114" display="shrushti.mulage@urbangabru.in" xr:uid="{6033AC21-F7BE-4E51-A959-D5962C670FA3}"/>
+    <hyperlink ref="D73" r:id="rId115" xr:uid="{D4FDC315-7B6D-4469-88E3-1589B741FE41}"/>
+    <hyperlink ref="I73" r:id="rId116" xr:uid="{C558B3C7-EBFE-4FB4-ADD6-6EB2E4AD0F9E}"/>
+    <hyperlink ref="I74" r:id="rId117" xr:uid="{D462771F-AC20-49C3-B70C-FA245A6B1D6F}"/>
+    <hyperlink ref="D36" r:id="rId118" xr:uid="{E91DE87D-A790-4838-8760-70C6AC703D98}"/>
+    <hyperlink ref="I75" r:id="rId119" xr:uid="{8AB72D72-B60D-4E53-A04A-507971B9D6C3}"/>
+    <hyperlink ref="D75" r:id="rId120" xr:uid="{FB78035B-3BB6-44E6-A168-E41DD27DB633}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3735,7 +3772,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>61</v>
@@ -3751,7 +3788,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>77</v>
@@ -3775,7 +3812,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>68</v>
@@ -3783,7 +3820,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>47</v>
@@ -3791,7 +3828,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>40</v>
@@ -3807,7 +3844,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>29</v>
@@ -3823,7 +3860,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>12</v>
@@ -3887,7 +3924,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>96</v>
@@ -3895,7 +3932,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>98</v>
@@ -3911,7 +3948,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>106</v>
@@ -3919,7 +3956,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>114</v>
@@ -3954,12 +3991,12 @@
         <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>71</v>
@@ -3991,7 +4028,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B33" t="s">
         <v>135</v>
@@ -3999,10 +4036,10 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B34" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4023,7 +4060,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>145</v>
@@ -4031,7 +4068,7 @@
     </row>
     <row r="38" spans="1:2" ht="76.5">
       <c r="A38" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>147</v>
@@ -4055,7 +4092,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>156</v>
@@ -4063,7 +4100,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>159</v>
@@ -4087,7 +4124,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>167</v>
@@ -4127,10 +4164,10 @@
     </row>
     <row r="50" spans="1:2" ht="76.5">
       <c r="A50" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:2">

</xml_diff>

<commit_message>
update: latest changes to Streamlit app
</commit_message>
<xml_diff>
--- a/reporting_hierarchy.xlsx
+++ b/reporting_hierarchy.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29423"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="320" documentId="11_254B45AE2BF66FFC05FC9890E2159AB6B2E0D67D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D532BEE2-D452-40DD-BFE6-2DA7C7ECD66D}"/>
+  <xr:revisionPtr revIDLastSave="350" documentId="11_254B45AE2BF66FFC05FC9890E2159AB6B2E0D67D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7FA3966-F7D5-4878-ADBA-BB4C8644C06D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="298">
   <si>
     <t>Employee No</t>
   </si>
@@ -443,6 +443,12 @@
   </si>
   <si>
     <t>Video Editor Associate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nisamuddin </t>
+  </si>
+  <si>
+    <t>nisamudheen.p@urbangabru.in</t>
   </si>
   <si>
     <t>Chirag Chavan</t>
@@ -618,15 +624,6 @@
     <t>hassaan.syed@urbangabru.in</t>
   </si>
   <si>
-    <t>Prajkta Bhosale</t>
-  </si>
-  <si>
-    <t>prajkta.bhosale@urbangabru.in</t>
-  </si>
-  <si>
-    <t>Content Writer Associate</t>
-  </si>
-  <si>
     <t>Janhavi Saywan</t>
   </si>
   <si>
@@ -651,12 +648,6 @@
     <t>Video Production Associate</t>
   </si>
   <si>
-    <t>Priya Saraswat</t>
-  </si>
-  <si>
-    <t>priya.saraswat@urbangabru.in</t>
-  </si>
-  <si>
     <t>Saniya Jilani Khan</t>
   </si>
   <si>
@@ -775,12 +766,6 @@
   </si>
   <si>
     <t>naman.babuta@urbangabru.in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nisamuddin </t>
-  </si>
-  <si>
-    <t>nisamudheen.p@urbangabru.in</t>
   </si>
   <si>
     <t>Video Lead</t>
@@ -842,6 +827,49 @@
     <t>ananya.gautam@urbangabru.in</t>
   </si>
   <si>
+    <t xml:space="preserve">Alefia </t>
+  </si>
+  <si>
+    <t>alefia.husain@urbangabru.in</t>
+  </si>
+  <si>
+    <t>Creative Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content Strategy Specialst </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natasha </t>
+  </si>
+  <si>
+    <t>natasha.surendran@urbangabru.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content writer Specialist </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shivani </t>
+  </si>
+  <si>
+    <t>shivani.bagul@urbangabru.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content Strategist Sr Associate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shamit </t>
+  </si>
+  <si>
+    <t>shamit.basode@urbangabru.in</t>
+  </si>
+  <si>
+    <t>AI Video Editor Senior Associate</t>
+  </si>
+  <si>
     <t>Avinash Desale</t>
   </si>
   <si>
@@ -925,7 +953,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -975,8 +1003,20 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Zoho_Puvi_Regular"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -989,8 +1029,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1028,12 +1074,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1049,6 +1147,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1354,14 +1473,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" workbookViewId="0">
-      <selection activeCell="J76" sqref="J76"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="34.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
@@ -2491,7 +2611,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" ht="15.75">
       <c r="A36" s="1">
         <v>461</v>
       </c>
@@ -2513,14 +2633,14 @@
       <c r="G36" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J36" s="1">
-        <v>154</v>
+      <c r="H36" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2531,19 +2651,19 @@
         <v>10</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>64</v>
@@ -2563,10 +2683,10 @@
         <v>10</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>25</v>
@@ -2595,10 +2715,10 @@
         <v>10</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>13</v>
@@ -2627,10 +2747,10 @@
         <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>25</v>
@@ -2639,7 +2759,7 @@
         <v>73</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>89</v>
@@ -2659,10 +2779,10 @@
         <v>10</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>13</v>
@@ -2671,7 +2791,7 @@
         <v>85</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>16</v>
@@ -2691,10 +2811,10 @@
         <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>25</v>
@@ -2703,7 +2823,7 @@
         <v>35</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>37</v>
@@ -2723,19 +2843,19 @@
         <v>10</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>64</v>
@@ -2755,10 +2875,10 @@
         <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>61</v>
@@ -2767,7 +2887,7 @@
         <v>134</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>94</v>
@@ -2779,7 +2899,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" ht="15.75">
       <c r="A45" s="1">
         <v>538</v>
       </c>
@@ -2787,10 +2907,10 @@
         <v>10</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>61</v>
@@ -2799,16 +2919,16 @@
         <v>134</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J45" s="1">
-        <v>154</v>
+        <v>163</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J45" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2819,10 +2939,10 @@
         <v>10</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>25</v>
@@ -2831,7 +2951,7 @@
         <v>73</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>89</v>
@@ -2851,10 +2971,10 @@
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>25</v>
@@ -2863,7 +2983,7 @@
         <v>73</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>89</v>
@@ -2883,10 +3003,10 @@
         <v>10</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>25</v>
@@ -2895,7 +3015,7 @@
         <v>35</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>37</v>
@@ -2915,10 +3035,10 @@
         <v>10</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>25</v>
@@ -2927,7 +3047,7 @@
         <v>26</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>116</v>
@@ -2947,10 +3067,10 @@
         <v>10</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>56</v>
@@ -2959,10 +3079,10 @@
         <v>57</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>55</v>
@@ -2979,10 +3099,10 @@
         <v>10</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>56</v>
@@ -2991,10 +3111,10 @@
         <v>57</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>55</v>
@@ -3017,13 +3137,13 @@
         <v>131</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>94</v>
@@ -3043,19 +3163,19 @@
         <v>10</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>64</v>
@@ -3075,10 +3195,10 @@
         <v>10</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>25</v>
@@ -3087,7 +3207,7 @@
         <v>73</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>89</v>
@@ -3107,19 +3227,19 @@
         <v>10</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>64</v>
@@ -3139,19 +3259,19 @@
         <v>10</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>64</v>
@@ -3171,10 +3291,10 @@
         <v>10</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>25</v>
@@ -3183,7 +3303,7 @@
         <v>73</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>89</v>
@@ -3197,48 +3317,48 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="1">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>134</v>
+        <v>35</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="J58" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>25</v>
@@ -3247,7 +3367,7 @@
         <v>35</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>37</v>
@@ -3259,242 +3379,242 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" ht="15.75">
       <c r="A60" s="1">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J60" s="1">
-        <v>156</v>
+        <v>201</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J60" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J61" s="1">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>134</v>
+        <v>35</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="J62" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1">
-        <v>652</v>
+        <v>663</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>10</v>
+        <v>208</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>207</v>
+        <v>35</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="J63" s="1">
-        <v>141</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1">
-        <v>653</v>
+        <v>666</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>10</v>
+        <v>208</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="J64" s="1">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75">
       <c r="A65" s="1">
-        <v>663</v>
+        <v>671</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J65" s="1">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>135</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J65" s="8">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75">
       <c r="A66" s="1">
-        <v>666</v>
+        <v>672</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J66" s="1">
-        <v>157</v>
+        <v>217</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J66" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="1">
-        <v>671</v>
+      <c r="A67">
+        <v>701</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
+      </c>
+      <c r="C67" t="s">
+        <v>64</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>217</v>
+        <v>65</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>61</v>
@@ -3502,8 +3622,8 @@
       <c r="F67" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G67" s="1" t="s">
-        <v>135</v>
+      <c r="G67" t="s">
+        <v>218</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>94</v>
@@ -3516,144 +3636,144 @@
       </c>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="1">
-        <v>672</v>
+      <c r="A68">
+        <v>705</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D68" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C68" t="s">
         <v>219</v>
       </c>
+      <c r="D68" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="E68" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J68" s="1">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1">
+        <v>448</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J69" s="1">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15.75">
+      <c r="A70" s="8">
+        <v>720</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G68" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J68" s="1">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69">
+      <c r="G70" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" t="s">
+        <v>64</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J70">
         <v>701</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C69" t="s">
-        <v>64</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E69" s="1" t="s">
+    </row>
+    <row r="71" spans="1:10" ht="15.75">
+      <c r="A71" s="8">
+        <v>717</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G69" t="s">
-        <v>221</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J69" s="1">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70">
-        <v>705</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C70" t="s">
-        <v>222</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J70" s="1">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="1">
-        <v>448</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J71" s="1">
-        <v>615</v>
+      <c r="G71" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J71" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75">
       <c r="A72" s="8">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D72" s="10" t="s">
+      <c r="D72" s="8" t="s">
         <v>227</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -3663,94 +3783,94 @@
         <v>134</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H72" t="s">
-        <v>64</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J72">
-        <v>701</v>
+        <v>217</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J72" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75">
       <c r="A73" s="8">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D73" s="8" t="s">
         <v>228</v>
       </c>
+      <c r="D73" s="9" t="s">
+        <v>229</v>
+      </c>
       <c r="E73" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>134</v>
+        <v>35</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H73" t="s">
-        <v>94</v>
+        <v>105</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J73" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.75">
       <c r="A74" s="8">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="H74" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="J74" s="1">
-        <v>154</v>
+        <v>425</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75">
       <c r="A75" s="8">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>25</v>
@@ -3759,7 +3879,7 @@
         <v>35</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>37</v>
@@ -3773,138 +3893,138 @@
     </row>
     <row r="76" spans="1:10" ht="15.75">
       <c r="A76" s="8">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="H76" t="s">
-        <v>69</v>
+        <v>154</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="J76" s="1">
-        <v>425</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15.75">
       <c r="A77" s="8">
-        <v>711</v>
+        <v>724</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D77" s="9" t="s">
         <v>237</v>
       </c>
+      <c r="D77" s="8" t="s">
+        <v>238</v>
+      </c>
       <c r="E77" s="1" t="s">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>37</v>
+        <v>239</v>
+      </c>
+      <c r="H77" t="s">
+        <v>130</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="J77" s="1">
-        <v>156</v>
+        <v>615</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15.75">
       <c r="A78" s="8">
-        <v>710</v>
+        <v>721</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>241</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J78" s="1">
-        <v>156</v>
+        <v>163</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J78" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15.75">
       <c r="A79" s="8">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>241</v>
+        <v>136</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>178</v>
+        <v>61</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="G79" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="H79" t="s">
-        <v>130</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="J79" s="1">
-        <v>615</v>
+      <c r="H79" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J79" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15.75">
       <c r="A80" s="8">
-        <v>721</v>
+        <v>727</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>243</v>
@@ -3913,50 +4033,50 @@
         <v>244</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>134</v>
+        <v>56</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>161</v>
+        <v>245</v>
       </c>
       <c r="H80" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="J80" s="1">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15.75">
       <c r="A81" s="8">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="D81" s="9" t="s">
         <v>246</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="H81" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H81" t="s">
         <v>94</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="I81" s="3" t="s">
         <v>43</v>
       </c>
       <c r="J81" s="1">
@@ -3965,42 +4085,42 @@
     </row>
     <row r="82" spans="1:10" ht="15.75">
       <c r="A82" s="8">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>57</v>
+        <v>25</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>250</v>
+        <v>148</v>
       </c>
       <c r="H82" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="J82" s="1">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15.75">
       <c r="A83" s="8">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>251</v>
@@ -4009,62 +4129,62 @@
         <v>252</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G83" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="G83" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="H83" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="J83" s="1">
-        <v>154</v>
+        <v>615</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15.75">
       <c r="A84" s="8">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="D84" s="9" t="s">
+      <c r="D84" s="8" t="s">
         <v>255</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>73</v>
+        <v>134</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="H84" t="s">
-        <v>89</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J84" s="1">
-        <v>158</v>
+        <v>163</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I84" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J84" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="15.75">
       <c r="A85" s="8">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>256</v>
@@ -4073,90 +4193,157 @@
         <v>257</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>178</v>
+        <v>25</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>129</v>
+        <v>26</v>
       </c>
       <c r="G85" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="H85" t="s">
+        <v>69</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J85" s="1">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="15.75">
+      <c r="A86" s="11">
+        <v>740</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C86" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="H85" t="s">
-        <v>130</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="J85" s="1">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="15.75">
-      <c r="A86" s="8">
-        <v>733</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C86" s="8" t="s">
+      <c r="D86" s="13" t="s">
         <v>259</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G86" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J86" s="1">
-        <v>154</v>
+      <c r="F86" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="H86" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J86" s="8">
+        <v>725</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="15.75">
-      <c r="A87" s="8">
-        <v>732</v>
+      <c r="A87" s="11">
+        <v>741</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D87" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C87" s="12" t="s">
         <v>262</v>
       </c>
+      <c r="D87" s="13" t="s">
+        <v>263</v>
+      </c>
       <c r="E87" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G87" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="H87" t="s">
-        <v>69</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J87" s="1">
-        <v>425</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I87" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J87" s="8">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="30.75">
+      <c r="A88" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F88" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J88" s="8">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="16.5">
+      <c r="A89" s="11">
+        <v>743</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="G89" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J89" s="8">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="15.75">
+      <c r="H90" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J89" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1" xr:uid="{638F569A-9090-47BA-ADB1-D610E608B36D}"/>
     <hyperlink ref="I4:I5" r:id="rId2" display="hemant.raulo@urbangabru.in" xr:uid="{F027F3A7-1A84-40C7-8699-209295903C83}"/>
@@ -4165,7 +4352,7 @@
     <hyperlink ref="I15" r:id="rId5" xr:uid="{E3CF6ABA-BCD4-4397-8765-1D319396C106}"/>
     <hyperlink ref="I24" r:id="rId6" xr:uid="{CEA99A94-15DC-48B6-B1F2-DE68A886F8FB}"/>
     <hyperlink ref="I31" r:id="rId7" xr:uid="{39A13FD4-080A-44B7-9F8C-94700230C307}"/>
-    <hyperlink ref="I63" r:id="rId8" xr:uid="{48A7FBF1-91F3-4040-B8DE-87501E505F2C}"/>
+    <hyperlink ref="I61" r:id="rId8" xr:uid="{48A7FBF1-91F3-4040-B8DE-87501E505F2C}"/>
     <hyperlink ref="I8" r:id="rId9" xr:uid="{DFAB2EC5-8C09-4564-B7BA-8382B61BFF14}"/>
     <hyperlink ref="D4" r:id="rId10" xr:uid="{C60DF700-70F7-44B2-8D62-554517801DFC}"/>
     <hyperlink ref="D50" r:id="rId11" xr:uid="{DA7D9228-82E2-4129-812D-193889E2BF35}"/>
@@ -4186,8 +4373,8 @@
     <hyperlink ref="I38" r:id="rId26" xr:uid="{EB64FEEB-BC2D-4126-8EE3-1834005CB9F7}"/>
     <hyperlink ref="I42" r:id="rId27" xr:uid="{096208DA-E231-4CEC-AFF9-826256C95D6A}"/>
     <hyperlink ref="I48" r:id="rId28" xr:uid="{A21CF0F9-3213-43D7-A413-7A257D8C0E50}"/>
-    <hyperlink ref="I59:I60" r:id="rId29" display="dhiraj.deshmukh@urbangabru.in" xr:uid="{97FB104B-C335-4156-BC01-9B9436223075}"/>
-    <hyperlink ref="I64:I65" r:id="rId30" display="dhiraj.deshmukh@urbangabru.in" xr:uid="{51BE2CCD-3E1C-40A1-B5D7-85090AED00A6}"/>
+    <hyperlink ref="I58:I59" r:id="rId29" display="dhiraj.deshmukh@urbangabru.in" xr:uid="{97FB104B-C335-4156-BC01-9B9436223075}"/>
+    <hyperlink ref="I62:I63" r:id="rId30" display="dhiraj.deshmukh@urbangabru.in" xr:uid="{51BE2CCD-3E1C-40A1-B5D7-85090AED00A6}"/>
     <hyperlink ref="D11" r:id="rId31" xr:uid="{02F65181-4C8F-42C4-902A-CDEE5F0647B6}"/>
     <hyperlink ref="I29" r:id="rId32" xr:uid="{C23024AB-ED52-41A8-A126-753C6738F61B}"/>
     <hyperlink ref="I49" r:id="rId33" xr:uid="{FBC8C4E5-4E75-43F4-BD96-B4259DFC017E}"/>
@@ -4195,101 +4382,95 @@
     <hyperlink ref="I50" r:id="rId35" xr:uid="{D230CE4C-4D5C-4742-A127-48601BB55C9F}"/>
     <hyperlink ref="I51" r:id="rId36" xr:uid="{CFD8CAD0-E3BB-4C26-B0B3-2476D05B3C82}"/>
     <hyperlink ref="I21" r:id="rId37" xr:uid="{4A21746D-8B08-4471-95F9-F2358AAFF29A}"/>
-    <hyperlink ref="I58" r:id="rId38" xr:uid="{AACCE424-ADF3-40DC-AF28-52F6A89CCA77}"/>
-    <hyperlink ref="I61:I62" r:id="rId39" display="arpita.achwal@urbangabru.in" xr:uid="{0DE873A0-BD9C-4A82-8F7A-F5C68EA0FEBB}"/>
-    <hyperlink ref="I67:I68" r:id="rId40" display="arpita.achwal@urbangabru.in" xr:uid="{82B181B4-78C8-4DF9-AD94-318490D08CA9}"/>
-    <hyperlink ref="D13" r:id="rId41" xr:uid="{7902939E-0487-48F1-84D7-CACB529741B0}"/>
-    <hyperlink ref="D14" r:id="rId42" xr:uid="{3AB174BA-7CED-4824-A663-6F227253BD9C}"/>
-    <hyperlink ref="D15" r:id="rId43" xr:uid="{A39FC705-BA1A-42C5-9955-53E724C009F5}"/>
-    <hyperlink ref="D16" r:id="rId44" xr:uid="{B63400E7-FA3C-4250-A756-02968FE61910}"/>
-    <hyperlink ref="D17" r:id="rId45" xr:uid="{D8735FC2-EC88-421B-8865-C4FE808C25EA}"/>
-    <hyperlink ref="D18" r:id="rId46" xr:uid="{A39D22E8-829E-408E-9A29-6AC69A125558}"/>
-    <hyperlink ref="D19" r:id="rId47" xr:uid="{C4514937-C1F9-4E05-9F4E-B78A90D5FF90}"/>
-    <hyperlink ref="D20" r:id="rId48" xr:uid="{7F8983E6-C30E-4371-83E6-E1BC55CAC1F9}"/>
-    <hyperlink ref="D21" r:id="rId49" xr:uid="{E0172095-1727-483E-9C84-789368420BFE}"/>
-    <hyperlink ref="D22" r:id="rId50" xr:uid="{80366AF4-50BC-4967-A78E-D47375491424}"/>
-    <hyperlink ref="D23" r:id="rId51" xr:uid="{F717CFC2-C0EF-434A-9B39-410B45E8DBF1}"/>
-    <hyperlink ref="D30" r:id="rId52" xr:uid="{564C77A2-C93C-41E3-92EE-584D1829ED3A}"/>
-    <hyperlink ref="I2" r:id="rId53" xr:uid="{C21C51C9-8E57-4306-AE33-5771DA9EDE44}"/>
-    <hyperlink ref="I16" r:id="rId54" xr:uid="{6A0113D1-0959-4068-A664-B46AA0B1D2D1}"/>
-    <hyperlink ref="I19" r:id="rId55" xr:uid="{3B003557-D297-4794-908F-89EC252AAA33}"/>
-    <hyperlink ref="I23" r:id="rId56" xr:uid="{F71DAFC5-7C60-446C-9821-205FEF06ADD1}"/>
-    <hyperlink ref="I27:I28" r:id="rId57" display="rakesh.raulo@urbangabru.in" xr:uid="{AB2C998F-9AAA-423C-B750-1494CDFA5F7C}"/>
-    <hyperlink ref="I39" r:id="rId58" xr:uid="{6AAF4B77-CA93-4DC8-8DAF-F80FD4448AC7}"/>
-    <hyperlink ref="I41" r:id="rId59" xr:uid="{AF208654-2826-41FA-AA0B-97B2CF2997E8}"/>
-    <hyperlink ref="I66" r:id="rId60" xr:uid="{462AE825-8F34-414D-BE17-BF41645E7288}"/>
-    <hyperlink ref="D31" r:id="rId61" xr:uid="{870AB10C-3CF3-4DDC-9EC0-B411812950CC}"/>
-    <hyperlink ref="D32" r:id="rId62" xr:uid="{B2402A95-78BF-4BCE-88CF-EB9D6A842F63}"/>
-    <hyperlink ref="D34" r:id="rId63" xr:uid="{2CB97427-98B8-49D0-ADE6-B829475893D2}"/>
-    <hyperlink ref="D37" r:id="rId64" xr:uid="{33D90B85-D89C-4BB2-B836-561FEABBF159}"/>
-    <hyperlink ref="D38" r:id="rId65" xr:uid="{16DF7F2F-BF7C-4CA7-8233-3C777EE637EF}"/>
-    <hyperlink ref="D39" r:id="rId66" xr:uid="{62BA3FE9-2B7D-4E82-A6AB-861684EE44FF}"/>
-    <hyperlink ref="D40" r:id="rId67" xr:uid="{9453D832-D2B1-4EA4-B67D-ED07B05CB36B}"/>
-    <hyperlink ref="D41" r:id="rId68" xr:uid="{4551821A-2077-4E19-8923-97622E114CC5}"/>
-    <hyperlink ref="D42" r:id="rId69" xr:uid="{80F5A021-7451-45CF-8A55-84C6B184D545}"/>
-    <hyperlink ref="D43" r:id="rId70" xr:uid="{823DA6B3-861B-4DDE-9318-3D9D9501A748}"/>
-    <hyperlink ref="D44" r:id="rId71" xr:uid="{57FB5EFB-0A7A-447E-B048-753DDCBE83BE}"/>
-    <hyperlink ref="D45" r:id="rId72" xr:uid="{65D20DC5-D347-4B92-939D-67C6E9CA4099}"/>
-    <hyperlink ref="D46" r:id="rId73" xr:uid="{DFDBB072-57B6-414E-AD32-C43529C0A02E}"/>
-    <hyperlink ref="D33" r:id="rId74" xr:uid="{F32CC1AB-1D08-4CBF-8734-41FE9CE792F2}"/>
-    <hyperlink ref="D36" r:id="rId75" xr:uid="{91939463-F347-4EB1-9835-10D0C5847AC2}"/>
-    <hyperlink ref="D48" r:id="rId76" xr:uid="{697A9CA5-37EE-4DA8-8785-23118AA9A986}"/>
-    <hyperlink ref="D49" r:id="rId77" xr:uid="{B837B941-6C09-4383-8340-057EFEEF4C2A}"/>
-    <hyperlink ref="D51" r:id="rId78" xr:uid="{5228BFFC-0024-4B76-A50F-378E909DEB9E}"/>
-    <hyperlink ref="D54" r:id="rId79" xr:uid="{03A49264-3529-4D46-96B4-F9E4B408275C}"/>
-    <hyperlink ref="D55" r:id="rId80" xr:uid="{B80B62FD-0A48-424D-9193-718DE528A3D9}"/>
-    <hyperlink ref="D57" r:id="rId81" xr:uid="{FF27CE65-EDD1-48CB-ADD2-FC1B04379D4F}"/>
-    <hyperlink ref="D58" r:id="rId82" xr:uid="{DD7177EA-B1A0-4A32-8ECC-126A8F698C87}"/>
-    <hyperlink ref="D59" r:id="rId83" xr:uid="{51AD824A-C8CC-4BDA-BDCB-CACD814337EE}"/>
-    <hyperlink ref="D60" r:id="rId84" xr:uid="{4D20B7EA-6506-4321-91D8-D043FDC215DB}"/>
-    <hyperlink ref="D61" r:id="rId85" xr:uid="{53CA0A1B-9838-4F34-9189-994827F11B4F}"/>
-    <hyperlink ref="D62" r:id="rId86" xr:uid="{006B567B-960D-4976-BA47-34C8AAC2EA6B}"/>
-    <hyperlink ref="D63" r:id="rId87" xr:uid="{D77DFDE8-52D1-47B3-937D-8875B12C8187}"/>
-    <hyperlink ref="D64" r:id="rId88" xr:uid="{4DAD1DCD-6DA4-4821-8767-096D23FA684C}"/>
-    <hyperlink ref="D65" r:id="rId89" xr:uid="{DE32128C-030C-49D8-B6C1-826E021812FC}"/>
-    <hyperlink ref="D66" r:id="rId90" xr:uid="{CBA88F32-2246-46B4-AC53-88544E823387}"/>
-    <hyperlink ref="D67" r:id="rId91" xr:uid="{FC846F3F-D1FA-4F31-B652-3CF29A90246C}"/>
-    <hyperlink ref="D68" r:id="rId92" xr:uid="{BFEFF04B-2141-4567-96A6-D3056766BB0D}"/>
-    <hyperlink ref="I35" r:id="rId93" xr:uid="{A6C0CC82-44BA-4222-B39E-D7476DA47C6B}"/>
-    <hyperlink ref="I14" r:id="rId94" xr:uid="{4C4DDAEE-F389-4B2E-BF3A-B7B53B7D3F87}"/>
-    <hyperlink ref="I33:I34" r:id="rId95" display="shailesh.bhujbal@urbangabru.co.in" xr:uid="{4B015309-8B52-4485-9965-99C88E6F4FAC}"/>
-    <hyperlink ref="I20" r:id="rId96" xr:uid="{E2E655CA-8855-4FFF-8D68-FE7BE3856DAD}"/>
-    <hyperlink ref="I22" r:id="rId97" xr:uid="{249F710E-612E-4A2B-9513-A7E0D75A00F0}"/>
-    <hyperlink ref="I30" r:id="rId98" xr:uid="{0DDB982B-4488-4CAE-AE51-CE129FB8AF5D}"/>
-    <hyperlink ref="I40" r:id="rId99" xr:uid="{6CE8AB3C-163D-40F6-96CD-419E037BC515}"/>
-    <hyperlink ref="I46:I47" r:id="rId100" xr:uid="{49138BDB-FD98-425A-8A09-D467631C7A6C}"/>
-    <hyperlink ref="I54" r:id="rId101" xr:uid="{85529956-96FD-44B7-B1B5-B8B96D656A21}"/>
-    <hyperlink ref="I57" r:id="rId102" xr:uid="{B3890C9C-5043-447C-9BE8-849115F9ED91}"/>
-    <hyperlink ref="I13" r:id="rId103" xr:uid="{B06B408B-86DE-4DC1-A0B1-E651C3474CC0}"/>
-    <hyperlink ref="D69" r:id="rId104" xr:uid="{2BB55C61-927A-4ACD-BFB5-8BFBEB3AB87D}"/>
-    <hyperlink ref="I69" r:id="rId105" xr:uid="{FE4CB666-8CCD-41A4-88DC-772F7E72B69E}"/>
-    <hyperlink ref="I18" r:id="rId106" xr:uid="{65D62495-7ED6-4AEE-85AA-5E06DD4DCC50}"/>
-    <hyperlink ref="I37" r:id="rId107" xr:uid="{5A19F303-21CE-4C85-8F0C-E1C79BC97EE4}"/>
-    <hyperlink ref="I43" r:id="rId108" xr:uid="{CE65FCF0-CAD9-4672-ABBE-37B0F48F2980}"/>
-    <hyperlink ref="I53" r:id="rId109" xr:uid="{EE4F0454-9D7B-4D12-AF17-1357CE1D3E35}"/>
-    <hyperlink ref="I55:I56" r:id="rId110" display="shrushti.mulage@urbangabru.in" xr:uid="{6033AC21-F7BE-4E51-A959-D5962C670FA3}"/>
-    <hyperlink ref="D70" r:id="rId111" xr:uid="{D4FDC315-7B6D-4469-88E3-1589B741FE41}"/>
-    <hyperlink ref="I70" r:id="rId112" xr:uid="{C558B3C7-EBFE-4FB4-ADD6-6EB2E4AD0F9E}"/>
-    <hyperlink ref="D35" r:id="rId113" xr:uid="{E91DE87D-A790-4838-8760-70C6AC703D98}"/>
-    <hyperlink ref="I71" r:id="rId114" xr:uid="{8AB72D72-B60D-4E53-A04A-507971B9D6C3}"/>
-    <hyperlink ref="D71" r:id="rId115" xr:uid="{FB78035B-3BB6-44E6-A168-E41DD27DB633}"/>
-    <hyperlink ref="D72" r:id="rId116" xr:uid="{99C33B73-DF8E-48F4-898C-A8EE9AFBA7F4}"/>
-    <hyperlink ref="I75" r:id="rId117" xr:uid="{D457B946-2C7C-4D94-BB76-75FC21CE52AE}"/>
-    <hyperlink ref="I77" r:id="rId118" xr:uid="{79D99990-0DCC-4038-95CC-DF502FDAB3FC}"/>
-    <hyperlink ref="I78" r:id="rId119" xr:uid="{89E8B74E-5421-47D4-81EB-28C833655F35}"/>
-    <hyperlink ref="I81" r:id="rId120" xr:uid="{91EAD886-D9E8-43C2-A469-FBD57EE676CD}"/>
-    <hyperlink ref="I79" r:id="rId121" xr:uid="{07B08EF3-2DC3-4B36-A0A4-AA3B13FD9442}"/>
-    <hyperlink ref="I85" r:id="rId122" xr:uid="{DBF62D72-BF4A-4175-AEE0-1A67E739CA4C}"/>
-    <hyperlink ref="I82" r:id="rId123" xr:uid="{3460E9AA-2796-472B-9A8C-201426F3C6E0}"/>
-    <hyperlink ref="I84" r:id="rId124" xr:uid="{17A1B2FB-8E41-4354-AEE2-2E9E5B0D2906}"/>
-    <hyperlink ref="I76" r:id="rId125" xr:uid="{5FA8D04A-7C92-467B-94EC-59E9AAF858F0}"/>
-    <hyperlink ref="I87" r:id="rId126" xr:uid="{4C626523-9255-4EE9-B00F-76F0973AB813}"/>
-    <hyperlink ref="I72" r:id="rId127" xr:uid="{C11183B9-2495-4806-B47C-D70E16538657}"/>
-    <hyperlink ref="I73" r:id="rId128" xr:uid="{AD8F2850-D134-4829-A85A-2BD289B20186}"/>
-    <hyperlink ref="I74" r:id="rId129" xr:uid="{403D12D0-12E0-43D5-A47F-365A9BE6811C}"/>
-    <hyperlink ref="I80" r:id="rId130" xr:uid="{F853E0B2-482A-4F07-8009-BC12BE6B115B}"/>
-    <hyperlink ref="I83" r:id="rId131" xr:uid="{390DE4D6-96FF-440B-9454-B84E3B267EA1}"/>
-    <hyperlink ref="I86" r:id="rId132" xr:uid="{74460AC2-C4F4-4242-8DA4-06BB68025728}"/>
+    <hyperlink ref="D13" r:id="rId38" xr:uid="{7902939E-0487-48F1-84D7-CACB529741B0}"/>
+    <hyperlink ref="D14" r:id="rId39" xr:uid="{3AB174BA-7CED-4824-A663-6F227253BD9C}"/>
+    <hyperlink ref="D15" r:id="rId40" xr:uid="{A39FC705-BA1A-42C5-9955-53E724C009F5}"/>
+    <hyperlink ref="D16" r:id="rId41" xr:uid="{B63400E7-FA3C-4250-A756-02968FE61910}"/>
+    <hyperlink ref="D17" r:id="rId42" xr:uid="{D8735FC2-EC88-421B-8865-C4FE808C25EA}"/>
+    <hyperlink ref="D18" r:id="rId43" xr:uid="{A39D22E8-829E-408E-9A29-6AC69A125558}"/>
+    <hyperlink ref="D19" r:id="rId44" xr:uid="{C4514937-C1F9-4E05-9F4E-B78A90D5FF90}"/>
+    <hyperlink ref="D20" r:id="rId45" xr:uid="{7F8983E6-C30E-4371-83E6-E1BC55CAC1F9}"/>
+    <hyperlink ref="D21" r:id="rId46" xr:uid="{E0172095-1727-483E-9C84-789368420BFE}"/>
+    <hyperlink ref="D22" r:id="rId47" xr:uid="{80366AF4-50BC-4967-A78E-D47375491424}"/>
+    <hyperlink ref="D23" r:id="rId48" xr:uid="{F717CFC2-C0EF-434A-9B39-410B45E8DBF1}"/>
+    <hyperlink ref="D30" r:id="rId49" xr:uid="{564C77A2-C93C-41E3-92EE-584D1829ED3A}"/>
+    <hyperlink ref="I2" r:id="rId50" xr:uid="{C21C51C9-8E57-4306-AE33-5771DA9EDE44}"/>
+    <hyperlink ref="I16" r:id="rId51" xr:uid="{6A0113D1-0959-4068-A664-B46AA0B1D2D1}"/>
+    <hyperlink ref="I19" r:id="rId52" xr:uid="{3B003557-D297-4794-908F-89EC252AAA33}"/>
+    <hyperlink ref="I23" r:id="rId53" xr:uid="{F71DAFC5-7C60-446C-9821-205FEF06ADD1}"/>
+    <hyperlink ref="I27:I28" r:id="rId54" display="rakesh.raulo@urbangabru.in" xr:uid="{AB2C998F-9AAA-423C-B750-1494CDFA5F7C}"/>
+    <hyperlink ref="I39" r:id="rId55" xr:uid="{6AAF4B77-CA93-4DC8-8DAF-F80FD4448AC7}"/>
+    <hyperlink ref="I41" r:id="rId56" xr:uid="{AF208654-2826-41FA-AA0B-97B2CF2997E8}"/>
+    <hyperlink ref="I64" r:id="rId57" xr:uid="{462AE825-8F34-414D-BE17-BF41645E7288}"/>
+    <hyperlink ref="D31" r:id="rId58" xr:uid="{870AB10C-3CF3-4DDC-9EC0-B411812950CC}"/>
+    <hyperlink ref="D32" r:id="rId59" xr:uid="{B2402A95-78BF-4BCE-88CF-EB9D6A842F63}"/>
+    <hyperlink ref="D34" r:id="rId60" xr:uid="{2CB97427-98B8-49D0-ADE6-B829475893D2}"/>
+    <hyperlink ref="D37" r:id="rId61" xr:uid="{33D90B85-D89C-4BB2-B836-561FEABBF159}"/>
+    <hyperlink ref="D38" r:id="rId62" xr:uid="{16DF7F2F-BF7C-4CA7-8233-3C777EE637EF}"/>
+    <hyperlink ref="D39" r:id="rId63" xr:uid="{62BA3FE9-2B7D-4E82-A6AB-861684EE44FF}"/>
+    <hyperlink ref="D40" r:id="rId64" xr:uid="{9453D832-D2B1-4EA4-B67D-ED07B05CB36B}"/>
+    <hyperlink ref="D41" r:id="rId65" xr:uid="{4551821A-2077-4E19-8923-97622E114CC5}"/>
+    <hyperlink ref="D42" r:id="rId66" xr:uid="{80F5A021-7451-45CF-8A55-84C6B184D545}"/>
+    <hyperlink ref="D43" r:id="rId67" xr:uid="{823DA6B3-861B-4DDE-9318-3D9D9501A748}"/>
+    <hyperlink ref="D44" r:id="rId68" xr:uid="{57FB5EFB-0A7A-447E-B048-753DDCBE83BE}"/>
+    <hyperlink ref="D45" r:id="rId69" xr:uid="{65D20DC5-D347-4B92-939D-67C6E9CA4099}"/>
+    <hyperlink ref="D46" r:id="rId70" xr:uid="{DFDBB072-57B6-414E-AD32-C43529C0A02E}"/>
+    <hyperlink ref="D33" r:id="rId71" xr:uid="{F32CC1AB-1D08-4CBF-8734-41FE9CE792F2}"/>
+    <hyperlink ref="D36" r:id="rId72" xr:uid="{91939463-F347-4EB1-9835-10D0C5847AC2}"/>
+    <hyperlink ref="D48" r:id="rId73" xr:uid="{697A9CA5-37EE-4DA8-8785-23118AA9A986}"/>
+    <hyperlink ref="D49" r:id="rId74" xr:uid="{B837B941-6C09-4383-8340-057EFEEF4C2A}"/>
+    <hyperlink ref="D51" r:id="rId75" xr:uid="{5228BFFC-0024-4B76-A50F-378E909DEB9E}"/>
+    <hyperlink ref="D54" r:id="rId76" xr:uid="{03A49264-3529-4D46-96B4-F9E4B408275C}"/>
+    <hyperlink ref="D55" r:id="rId77" xr:uid="{B80B62FD-0A48-424D-9193-718DE528A3D9}"/>
+    <hyperlink ref="D57" r:id="rId78" xr:uid="{FF27CE65-EDD1-48CB-ADD2-FC1B04379D4F}"/>
+    <hyperlink ref="D58" r:id="rId79" xr:uid="{51AD824A-C8CC-4BDA-BDCB-CACD814337EE}"/>
+    <hyperlink ref="D59" r:id="rId80" xr:uid="{4D20B7EA-6506-4321-91D8-D043FDC215DB}"/>
+    <hyperlink ref="D60" r:id="rId81" xr:uid="{53CA0A1B-9838-4F34-9189-994827F11B4F}"/>
+    <hyperlink ref="D61" r:id="rId82" xr:uid="{D77DFDE8-52D1-47B3-937D-8875B12C8187}"/>
+    <hyperlink ref="D62" r:id="rId83" xr:uid="{4DAD1DCD-6DA4-4821-8767-096D23FA684C}"/>
+    <hyperlink ref="D63" r:id="rId84" xr:uid="{DE32128C-030C-49D8-B6C1-826E021812FC}"/>
+    <hyperlink ref="D64" r:id="rId85" xr:uid="{CBA88F32-2246-46B4-AC53-88544E823387}"/>
+    <hyperlink ref="D65" r:id="rId86" xr:uid="{FC846F3F-D1FA-4F31-B652-3CF29A90246C}"/>
+    <hyperlink ref="D66" r:id="rId87" xr:uid="{BFEFF04B-2141-4567-96A6-D3056766BB0D}"/>
+    <hyperlink ref="I35" r:id="rId88" xr:uid="{A6C0CC82-44BA-4222-B39E-D7476DA47C6B}"/>
+    <hyperlink ref="I14" r:id="rId89" xr:uid="{4C4DDAEE-F389-4B2E-BF3A-B7B53B7D3F87}"/>
+    <hyperlink ref="I33:I34" r:id="rId90" display="shailesh.bhujbal@urbangabru.co.in" xr:uid="{4B015309-8B52-4485-9965-99C88E6F4FAC}"/>
+    <hyperlink ref="I20" r:id="rId91" xr:uid="{E2E655CA-8855-4FFF-8D68-FE7BE3856DAD}"/>
+    <hyperlink ref="I22" r:id="rId92" xr:uid="{249F710E-612E-4A2B-9513-A7E0D75A00F0}"/>
+    <hyperlink ref="I30" r:id="rId93" xr:uid="{0DDB982B-4488-4CAE-AE51-CE129FB8AF5D}"/>
+    <hyperlink ref="I40" r:id="rId94" xr:uid="{6CE8AB3C-163D-40F6-96CD-419E037BC515}"/>
+    <hyperlink ref="I46:I47" r:id="rId95" xr:uid="{49138BDB-FD98-425A-8A09-D467631C7A6C}"/>
+    <hyperlink ref="I54" r:id="rId96" xr:uid="{85529956-96FD-44B7-B1B5-B8B96D656A21}"/>
+    <hyperlink ref="I57" r:id="rId97" xr:uid="{B3890C9C-5043-447C-9BE8-849115F9ED91}"/>
+    <hyperlink ref="I13" r:id="rId98" xr:uid="{B06B408B-86DE-4DC1-A0B1-E651C3474CC0}"/>
+    <hyperlink ref="D67" r:id="rId99" xr:uid="{2BB55C61-927A-4ACD-BFB5-8BFBEB3AB87D}"/>
+    <hyperlink ref="I67" r:id="rId100" xr:uid="{FE4CB666-8CCD-41A4-88DC-772F7E72B69E}"/>
+    <hyperlink ref="I18" r:id="rId101" xr:uid="{65D62495-7ED6-4AEE-85AA-5E06DD4DCC50}"/>
+    <hyperlink ref="I37" r:id="rId102" xr:uid="{5A19F303-21CE-4C85-8F0C-E1C79BC97EE4}"/>
+    <hyperlink ref="I43" r:id="rId103" xr:uid="{CE65FCF0-CAD9-4672-ABBE-37B0F48F2980}"/>
+    <hyperlink ref="I53" r:id="rId104" xr:uid="{EE4F0454-9D7B-4D12-AF17-1357CE1D3E35}"/>
+    <hyperlink ref="I55:I56" r:id="rId105" display="shrushti.mulage@urbangabru.in" xr:uid="{6033AC21-F7BE-4E51-A959-D5962C670FA3}"/>
+    <hyperlink ref="D68" r:id="rId106" xr:uid="{D4FDC315-7B6D-4469-88E3-1589B741FE41}"/>
+    <hyperlink ref="I68" r:id="rId107" xr:uid="{C558B3C7-EBFE-4FB4-ADD6-6EB2E4AD0F9E}"/>
+    <hyperlink ref="D35" r:id="rId108" xr:uid="{E91DE87D-A790-4838-8760-70C6AC703D98}"/>
+    <hyperlink ref="I69" r:id="rId109" xr:uid="{8AB72D72-B60D-4E53-A04A-507971B9D6C3}"/>
+    <hyperlink ref="D69" r:id="rId110" xr:uid="{FB78035B-3BB6-44E6-A168-E41DD27DB633}"/>
+    <hyperlink ref="D70" r:id="rId111" xr:uid="{99C33B73-DF8E-48F4-898C-A8EE9AFBA7F4}"/>
+    <hyperlink ref="I73" r:id="rId112" xr:uid="{D457B946-2C7C-4D94-BB76-75FC21CE52AE}"/>
+    <hyperlink ref="I75" r:id="rId113" xr:uid="{79D99990-0DCC-4038-95CC-DF502FDAB3FC}"/>
+    <hyperlink ref="I76" r:id="rId114" xr:uid="{89E8B74E-5421-47D4-81EB-28C833655F35}"/>
+    <hyperlink ref="I77" r:id="rId115" xr:uid="{07B08EF3-2DC3-4B36-A0A4-AA3B13FD9442}"/>
+    <hyperlink ref="I83" r:id="rId116" xr:uid="{DBF62D72-BF4A-4175-AEE0-1A67E739CA4C}"/>
+    <hyperlink ref="I80" r:id="rId117" xr:uid="{3460E9AA-2796-472B-9A8C-201426F3C6E0}"/>
+    <hyperlink ref="I82" r:id="rId118" xr:uid="{17A1B2FB-8E41-4354-AEE2-2E9E5B0D2906}"/>
+    <hyperlink ref="I74" r:id="rId119" xr:uid="{5FA8D04A-7C92-467B-94EC-59E9AAF858F0}"/>
+    <hyperlink ref="I85" r:id="rId120" xr:uid="{4C626523-9255-4EE9-B00F-76F0973AB813}"/>
+    <hyperlink ref="I70" r:id="rId121" xr:uid="{C11183B9-2495-4806-B47C-D70E16538657}"/>
+    <hyperlink ref="I81" r:id="rId122" xr:uid="{390DE4D6-96FF-440B-9454-B84E3B267EA1}"/>
+    <hyperlink ref="D86" r:id="rId123" xr:uid="{5921F1F7-B8A1-4782-A970-58A9CE9F4724}"/>
+    <hyperlink ref="D87" r:id="rId124" xr:uid="{D3136A9D-F831-4278-BC8A-A868CD17A8D1}"/>
+    <hyperlink ref="D88" r:id="rId125" xr:uid="{118D3B29-FAC4-4608-8C12-BF22A4DE7E59}"/>
+    <hyperlink ref="D89" r:id="rId126" xr:uid="{A10E8DDF-9A5C-4E28-B049-98A52B6962CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4311,7 +4492,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>60</v>
@@ -4327,7 +4508,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>76</v>
@@ -4351,7 +4532,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>67</v>
@@ -4359,7 +4540,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>47</v>
@@ -4367,7 +4548,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>40</v>
@@ -4383,7 +4564,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>29</v>
@@ -4399,7 +4580,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>12</v>
@@ -4463,15 +4644,15 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>96</v>
@@ -4487,7 +4668,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>104</v>
@@ -4495,7 +4676,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>112</v>
@@ -4530,12 +4711,12 @@
         <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>70</v>
@@ -4567,7 +4748,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="B33" t="s">
         <v>133</v>
@@ -4575,154 +4756,154 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="B34" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="76.5">
       <c r="A38" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="76.5">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="76.5">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="76.5">
       <c r="A50" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="76.5">
       <c r="A52" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>